<commit_message>
updated region3 station file list
</commit_message>
<xml_diff>
--- a/config/Region3_Stations_V1.xlsx
+++ b/config/Region3_Stations_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanton/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanton/GitHub/RENCI/ADCIRCSupportTools/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B357AE8-5D83-8D49-BE96-FBDBDCCFDAD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB32426E-D3B5-8E49-B4F3-50AC870A53A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="33040" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="-20880" windowWidth="25280" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region3_Stations_V1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="98">
   <si>
     <t>serial_nr</t>
   </si>
@@ -300,6 +300,21 @@
   </si>
   <si>
     <t>South Padre Island Coast Guard Station</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>bathy</t>
+  </si>
+  <si>
+    <t>element</t>
+  </si>
+  <si>
+    <t>node</t>
   </si>
 </sst>
 </file>
@@ -445,7 +460,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +646,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -792,13 +813,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1156,14 +1179,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="11" max="11" width="20.6640625" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -1198,19 +1222,19 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1871,98 +1895,98 @@
         <v>879383</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:15" s="6" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
         <v>8534720</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16">
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6">
         <v>-74.418300000000002</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="6">
         <v>39.354999999999997</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="6">
         <v>0.4</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="6">
         <v>0.12189999999999999</v>
       </c>
-      <c r="J16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="2">
-        <v>-74.400000000000006</v>
-      </c>
-      <c r="L16" s="2">
-        <v>39.4</v>
-      </c>
-      <c r="M16">
+      <c r="J16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="7">
+        <v>-74.4025129999999</v>
+      </c>
+      <c r="L16" s="7">
+        <v>39.397917</v>
+      </c>
+      <c r="M16" s="6">
         <v>3.3689</v>
       </c>
-      <c r="N16">
-        <v>1942291</v>
-      </c>
-      <c r="O16">
-        <v>1025264</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="N16" s="6">
+        <v>2062198</v>
+      </c>
+      <c r="O16" s="6">
+        <v>1029550</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="6">
         <v>8536110</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17">
+      <c r="E17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="6">
         <v>-74.959999999999994</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="6">
         <v>38.968330000000002</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="6">
         <v>0.45</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="6">
         <v>0.13719999999999999</v>
       </c>
-      <c r="J17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="2">
-        <v>-74.963659000000007</v>
-      </c>
-      <c r="L17" s="2">
-        <v>38.969112000000003</v>
-      </c>
-      <c r="M17">
+      <c r="J17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="7">
+        <v>-74.964130999999895</v>
+      </c>
+      <c r="L17" s="7">
+        <v>38.969316999999997</v>
+      </c>
+      <c r="M17" s="6">
         <v>0.47660000000000002</v>
       </c>
-      <c r="N17">
-        <v>144213</v>
-      </c>
-      <c r="O17">
-        <v>73322</v>
+      <c r="N17" s="6">
+        <v>144255</v>
+      </c>
+      <c r="O17" s="6">
+        <v>72229</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -2294,51 +2318,51 @@
         <v>927369</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4">
+    <row r="25" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6">
         <v>8661070</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="E25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="6">
         <v>-78.916383999999994</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="6">
         <v>33.655000000000001</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="6">
         <v>0.45</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="6">
         <v>0.13719999999999999</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="5">
-        <v>-78.916383999999994</v>
-      </c>
-      <c r="L25" s="5">
-        <v>33.655000000000001</v>
-      </c>
-      <c r="M25" s="4">
+      <c r="J25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="7">
+        <v>-78.909931</v>
+      </c>
+      <c r="L25" s="7">
+        <v>33.641724000000004</v>
+      </c>
+      <c r="M25" s="6">
         <v>7.0872999999999999</v>
       </c>
-      <c r="N25" s="4">
+      <c r="N25" s="6">
         <v>1840490</v>
       </c>
-      <c r="O25" s="4">
-        <v>917914</v>
+      <c r="O25" s="6">
+        <v>913115</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2456,6 +2480,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adjusted Atl City and Cape May node indices
</commit_message>
<xml_diff>
--- a/config/Region3_Stations_V1.xlsx
+++ b/config/Region3_Stations_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanton/GitHub/RENCI/ADCIRCSupportTools/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01274C85-7E91-6741-91BD-4D019429A38D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08C32BB-CA7C-5B4E-85EF-771BC1CF2DF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="-20880" windowWidth="25280" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="33040" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region3_Stations_V1" sheetId="1" r:id="rId1"/>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1927,66 +1927,66 @@
         <v>23</v>
       </c>
       <c r="K16" s="7">
-        <v>-74.4025129999999</v>
+        <v>-74.418297269295806</v>
       </c>
       <c r="L16" s="7">
-        <v>39.397917</v>
+        <v>39.3567908537158</v>
       </c>
       <c r="M16" s="6">
         <v>3.3689</v>
       </c>
       <c r="N16" s="6">
-        <v>2062198</v>
+        <v>1942291</v>
       </c>
       <c r="O16" s="6">
-        <v>1029550</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+        <v>964479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>8536110</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="E17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="4">
         <v>-74.959999999999994</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="4">
         <v>38.968330000000002</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="4">
         <v>0.45</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="4">
         <v>0.13719999999999999</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="7">
-        <v>-74.964130999999895</v>
-      </c>
-      <c r="L17" s="7">
-        <v>38.969316999999997</v>
-      </c>
-      <c r="M17" s="6">
+      <c r="J17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="5">
+        <v>-74.959962000000004</v>
+      </c>
+      <c r="L17" s="5">
+        <v>38.967747000000003</v>
+      </c>
+      <c r="M17" s="4">
         <v>0.47660000000000002</v>
       </c>
-      <c r="N17" s="6">
-        <v>144255</v>
-      </c>
-      <c r="O17" s="6">
-        <v>72229</v>
+      <c r="N17" s="4">
+        <v>144964</v>
+      </c>
+      <c r="O17" s="4">
+        <v>72477</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -2318,50 +2318,50 @@
         <v>927369</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>23</v>
-      </c>
-      <c r="B25" s="6">
+    <row r="25" spans="1:15" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
         <v>8661070</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="E25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="4">
         <v>-78.916383999999994</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="4">
         <v>33.655000000000001</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="4">
         <v>0.45</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="4">
         <v>0.13719999999999999</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="7">
+      <c r="J25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="5">
         <v>-78.909931</v>
       </c>
-      <c r="L25" s="7">
+      <c r="L25" s="5">
         <v>33.641724000000004</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25" s="4">
         <v>7.0872999999999999</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N25" s="4">
         <v>1840490</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="4">
         <v>913115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusted Beaufort node index
</commit_message>
<xml_diff>
--- a/config/Region3_Stations_V1.xlsx
+++ b/config/Region3_Stations_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanton/GitHub/RENCI/ADCIRCSupportTools/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08C32BB-CA7C-5B4E-85EF-771BC1CF2DF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5892EED-76C8-D649-BA19-F10C7A6EF214}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="33040" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,7 +648,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1179,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1895,50 +1895,50 @@
         <v>879383</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="6" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+    <row r="16" spans="1:15" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>8534720</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="E16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="4">
         <v>-74.418300000000002</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="4">
         <v>39.354999999999997</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="4">
         <v>0.4</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="4">
         <v>0.12189999999999999</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="7">
+      <c r="J16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="5">
         <v>-74.418297269295806</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="5">
         <v>39.3567908537158</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="4">
         <v>3.3689</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="4">
         <v>1942291</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="4">
         <v>964479</v>
       </c>
     </row>
@@ -2224,51 +2224,51 @@
         <v>876307</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <v>8656483</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23">
+      <c r="E23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="6">
         <v>-76.67</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="6">
         <v>34.72</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="6">
         <v>0.37</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="6">
         <v>0.1128</v>
       </c>
-      <c r="J23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="2">
-        <v>-76.671000000000006</v>
-      </c>
-      <c r="L23" s="2">
-        <v>34.72</v>
-      </c>
-      <c r="M23">
+      <c r="J23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="7">
+        <v>-76.672932000000003</v>
+      </c>
+      <c r="L23" s="7">
+        <v>13.52</v>
+      </c>
+      <c r="M23" s="6">
         <v>2.1093999999999999</v>
       </c>
-      <c r="N23">
-        <v>1868682</v>
-      </c>
-      <c r="O23">
-        <v>927421</v>
+      <c r="N23" s="6">
+        <v>1840640</v>
+      </c>
+      <c r="O23" s="6">
+        <v>917990</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated region3 station list for Delaware Bay; renamed clamp and control files
</commit_message>
<xml_diff>
--- a/config/Region3_Stations_V1.xlsx
+++ b/config/Region3_Stations_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanton/GitHub/RENCI/ADCIRCSupportTools/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DE479F-273A-7343-B244-5E934E8190AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C90A97C-9772-894F-BB40-C41169490624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11000" yWindow="-25580" windowWidth="37020" windowHeight="25580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-340" yWindow="-26160" windowWidth="37020" windowHeight="25580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region3_Stations_V1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="200">
   <si>
     <t>serial_nr</t>
   </si>
@@ -656,6 +656,9 @@
   </si>
   <si>
     <t>AG</t>
+  </si>
+  <si>
+    <t>Brandywine Shoal Light</t>
   </si>
 </sst>
 </file>
@@ -665,7 +668,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -811,6 +814,19 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1160,7 +1176,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1184,6 +1200,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1543,1306 +1567,1432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="2"/>
-    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="15"/>
+    <col min="3" max="3" width="25.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="10.83203125" style="15"/>
+    <col min="11" max="11" width="20.6640625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="16"/>
+    <col min="13" max="13" width="10.83203125" style="15"/>
+    <col min="14" max="14" width="12.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="15">
         <v>8410140</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="15">
         <v>-66.982315</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="15">
         <v>44.903300000000002</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="15">
         <v>0.23</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="15">
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="16">
         <v>-66.982315</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="16">
         <v>44.903300000000002</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="15">
         <v>36.701000000000001</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="15">
         <v>2113761</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="15">
         <v>1051378</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="15">
+        <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="15">
         <v>8413320</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="15">
         <v>-68.204999999999998</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="15">
         <v>44.3917</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="15">
         <v>0.27600000000000002</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="15">
         <v>8.4099999999999994E-2</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="16">
         <v>-68.169640000000001</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="16">
         <v>44.337400000000002</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="15">
         <v>4.5781999999999998</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="15">
         <v>1924278</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="15">
         <v>960216</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="15">
+        <f t="shared" ref="A5:A30" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="15">
         <v>8418150</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="15">
         <v>-70.245673999999994</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="15">
         <v>43.656700000000001</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="15">
         <v>0.32</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="15">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="16">
         <v>-70.198746999999997</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="16">
         <v>43.623342999999998</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="15">
         <v>11.305</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="15">
         <v>2028083</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="15">
         <v>1012396</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="15">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
         <v>8419317</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="15">
         <v>-70.563310000000001</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="15">
         <v>43.32</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="15">
         <v>0.37</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="15">
         <v>0.1128</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="16">
         <v>-70.556364000000002</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="16">
         <v>43.319060999999998</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="15">
         <v>1.6825000000000001</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="15">
         <v>2247942</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="15">
         <v>1778634</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="15">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="15">
         <v>8443970</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="15">
         <v>-71.038380000000004</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="15">
         <v>42.353920000000002</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="15">
         <v>0.3</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="15">
         <v>9.1399999999999995E-2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="16">
         <v>-70.959027000000006</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="16">
         <v>42.338478000000002</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="15">
         <v>12.382</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="15">
         <v>2257311</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="15">
         <v>1783467</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="15">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="15">
         <v>8447930</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="15">
         <v>-70.671700000000001</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="15">
         <v>41.523299999999999</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="15">
         <v>0.38</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="15">
         <v>0.1158</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="16">
         <v>-70.671700000000001</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="16">
         <v>41.523299999999999</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="15">
         <v>3.7334999999999998</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="15">
         <v>1831631</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="15">
         <v>908778</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="15">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="15">
         <v>8449130</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="15">
         <v>-70.091285999999997</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="15">
         <v>41.284999999999997</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="15">
         <v>0.26740000000000003</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="15">
         <v>8.1500000000000003E-2</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="16">
         <v>-70.096596000000005</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="16">
         <v>41.306587999999998</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="15">
         <v>4.8158000000000003</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="15">
         <v>1758010</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="15">
         <v>871780</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="15">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="15">
         <v>8461490</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="15">
         <v>-72.086699999999993</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="15">
         <v>41.354999999999997</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="15">
         <v>0.3</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="15">
         <v>9.1399999999999995E-2</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="16">
         <v>-72.071372999999994</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="16">
         <v>41.303212000000002</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="15">
         <v>8.1685999999999996</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="15">
         <v>1944826</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="15">
         <v>975291</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="15">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="15">
         <v>8465705</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="15">
         <v>-72.908299999999997</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="15">
         <v>41.283299999999997</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="15">
         <v>0.3553</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="15">
         <v>0.10829999999999999</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="16">
         <v>-72.915965999999997</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="16">
         <v>41.248365</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="15">
         <v>3.5746000000000002</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="15">
         <v>2262182</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="15">
         <v>1786035</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="15">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="15">
         <v>8467150</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="15">
         <v>-73.181700000000006</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="15">
         <v>41.173299999999998</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="15">
         <v>0.22</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="15">
         <v>6.7100000000000007E-2</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="16">
         <v>-73.180396000000002</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="16">
         <v>41.158848999999996</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="15">
         <v>5.5156000000000001</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="15">
         <v>2289722</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="15">
         <v>1136533</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="15">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="15">
         <v>8510560</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="15">
         <v>-71.959999999999994</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="15">
         <v>41.048299999999998</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="15">
         <v>0.33</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="15">
         <v>0.10059999999999999</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="16">
         <v>-71.979363000000006</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="16">
         <v>41.054951000000003</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="15">
         <v>4.4606000000000003</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="15">
         <v>1858329</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="15">
         <v>922825</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="15">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="15">
         <v>8516945</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="15">
         <v>-73.767882999999998</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="15">
         <v>40.810310000000001</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="15">
         <v>0.27</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="15">
         <v>8.2299999999999998E-2</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="16">
         <v>-73.767882999999998</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="16">
         <v>40.810310000000001</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="15">
         <v>7.1101000000000001</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="15">
         <v>2475973</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="15">
         <v>1227099</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="15">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="15">
         <v>8531680</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="15">
         <v>-74.010000000000005</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="15">
         <v>40.466700000000003</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="15">
         <v>0.24</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="15">
         <v>7.3099999999999998E-2</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="16">
         <v>-74</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="16">
         <v>40.5</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="15">
         <v>2.9794999999999998</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="15">
         <v>1782474</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="15">
         <v>879383</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+    <row r="16" spans="1:15" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="17">
         <v>8534720</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="17">
         <v>-74.418300000000002</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="17">
         <v>39.354999999999997</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="17">
         <v>0.4</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="17">
         <v>0.12189999999999999</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="18">
         <v>-74.418297269295806</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="18">
         <v>39.3567908537158</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="17">
         <v>3.3689</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16" s="17">
         <v>1942291</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16" s="17">
         <v>964479</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+    <row r="17" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="17">
         <v>8536110</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="17">
         <v>-74.959999999999994</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="17">
         <v>38.968330000000002</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="17">
         <v>0.45</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="17">
         <v>0.13719999999999999</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="18">
         <v>-74.959962000000004</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="18">
         <v>38.967747000000003</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="17">
         <v>0.47660000000000002</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="17">
         <v>144964</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="17">
         <v>72477</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="19">
+        <v>8555889</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="17">
+        <v>-75.113</v>
+      </c>
+      <c r="G18" s="17">
+        <v>38.987000000000002</v>
+      </c>
+      <c r="H18" s="17">
+        <v>0.42</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0.1313</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="17">
+        <v>-75.113</v>
+      </c>
+      <c r="L18" s="17">
+        <v>38.987000000000002</v>
+      </c>
+      <c r="M18" s="17">
+        <v>5</v>
+      </c>
+      <c r="N18" s="17">
+        <v>951064</v>
+      </c>
+      <c r="O18" s="17">
+        <v>477738</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="21">
+        <v>8551762</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="20">
+        <v>-75.571667000000005</v>
+      </c>
+      <c r="G19" s="20">
+        <v>39.558329999999998</v>
+      </c>
+      <c r="H19" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I19" s="20">
+        <v>0.12189999999999999</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="20">
+        <v>-75.571899999999999</v>
+      </c>
+      <c r="L19" s="20">
+        <v>39.558799999999998</v>
+      </c>
+      <c r="M19" s="20">
+        <v>8.98</v>
+      </c>
+      <c r="N19" s="20">
+        <v>14633</v>
+      </c>
+      <c r="O19" s="20">
+        <v>7231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="15">
         <v>8557380</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F18">
+      <c r="F20" s="15">
         <v>-75.119159999999994</v>
       </c>
-      <c r="G18">
+      <c r="G20" s="15">
         <v>38.785755999999999</v>
       </c>
-      <c r="H18">
+      <c r="H20" s="15">
         <v>0.4</v>
       </c>
-      <c r="I18">
+      <c r="I20" s="15">
         <v>0.12189999999999999</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J20" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K20" s="16">
         <v>-75.119159999999994</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L20" s="16">
         <v>38.785755999999999</v>
       </c>
-      <c r="M18">
+      <c r="M20" s="15">
         <v>3.7157</v>
       </c>
-      <c r="N18">
+      <c r="N20" s="15">
         <v>809492</v>
       </c>
-      <c r="O18">
+      <c r="O20" s="15">
         <v>406904</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="15">
         <v>8570283</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F19">
+      <c r="F21" s="15">
         <v>-75.091669999999993</v>
       </c>
-      <c r="G19">
+      <c r="G21" s="15">
         <v>38.328330000000001</v>
       </c>
-      <c r="H19">
+      <c r="H21" s="15">
         <v>0.36</v>
       </c>
-      <c r="I19">
+      <c r="I21" s="15">
         <v>0.10970000000000001</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J21" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K21" s="16">
         <v>-75.091669999999993</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L21" s="16">
         <v>38.328330000000001</v>
       </c>
-      <c r="M19">
+      <c r="M21" s="15">
         <v>3.0895000000000001</v>
       </c>
-      <c r="N19">
+      <c r="N21" s="15">
         <v>98824</v>
       </c>
-      <c r="O19">
+      <c r="O21" s="15">
         <v>49664</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="15">
         <v>8635750</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F20">
+      <c r="F22" s="15">
         <v>-76.464439999999996</v>
       </c>
-      <c r="G20">
+      <c r="G22" s="15">
         <v>37.996110000000002</v>
       </c>
-      <c r="H20">
+      <c r="H22" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I20">
+      <c r="I22" s="15">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K22" s="16">
         <v>-76.5</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L22" s="16">
         <v>38</v>
       </c>
-      <c r="M20">
+      <c r="M22" s="15">
         <v>2.2271999999999998</v>
       </c>
-      <c r="N20">
+      <c r="N22" s="15">
         <v>1713364</v>
       </c>
-      <c r="O20">
+      <c r="O22" s="15">
         <v>920362</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="15">
         <v>8638901</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F21">
+      <c r="F23" s="15">
         <v>-76.083332999999996</v>
       </c>
-      <c r="G21">
+      <c r="G23" s="15">
         <v>37.033332999999999</v>
       </c>
-      <c r="H21">
+      <c r="H23" s="15">
         <v>0.42099999999999999</v>
       </c>
-      <c r="I21">
+      <c r="I23" s="15">
         <v>0.1283</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K23" s="16">
         <v>-76.083332999999996</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L23" s="16">
         <v>37.033332999999999</v>
       </c>
-      <c r="M21">
+      <c r="M23" s="15">
         <v>12.99</v>
       </c>
-      <c r="N21">
+      <c r="N23" s="15">
         <v>2917097</v>
       </c>
-      <c r="O21">
+      <c r="O23" s="15">
         <v>1861105</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="15">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="15">
         <v>8651370</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F22">
+      <c r="F24" s="15">
         <v>-75.746669999999995</v>
       </c>
-      <c r="G22">
+      <c r="G24" s="15">
         <v>36.183329999999998</v>
       </c>
-      <c r="H22">
+      <c r="H24" s="15">
         <v>0.42</v>
       </c>
-      <c r="I22">
+      <c r="I24" s="15">
         <v>0.128</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K24" s="16">
         <v>-75.746669999999995</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L24" s="16">
         <v>36.183329999999998</v>
       </c>
-      <c r="M22">
+      <c r="M24" s="15">
         <v>3.4687000000000001</v>
       </c>
-      <c r="N22">
+      <c r="N24" s="15">
         <v>1767335</v>
       </c>
-      <c r="O22">
+      <c r="O24" s="15">
         <v>876307</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>21</v>
-      </c>
-      <c r="B23" s="4">
+    <row r="25" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="17">
         <v>8656483</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C25" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D25" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F25" s="17">
         <v>-76.67</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G25" s="17">
         <v>34.72</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H25" s="17">
         <v>0.37</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I25" s="17">
         <v>0.1128</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J25" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K25" s="18">
         <v>-76.672932000000003</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L25" s="18">
         <v>34.699781000000002</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M25" s="17">
         <v>2.1093999999999999</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N25" s="17">
         <v>1840640</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O25" s="17">
         <v>917990</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="15">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="15">
+        <v>8658163</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>8658163</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F26" s="15">
+        <v>-77.784972999999994</v>
+      </c>
+      <c r="G26" s="15">
+        <v>34.21331</v>
+      </c>
+      <c r="H26" s="15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0.17069999999999999</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="16">
+        <v>-77.784972999999994</v>
+      </c>
+      <c r="L26" s="16">
+        <v>34.21331</v>
+      </c>
+      <c r="M26" s="15">
+        <v>2.5758999999999999</v>
+      </c>
+      <c r="N26" s="15">
+        <v>1859231</v>
+      </c>
+      <c r="O26" s="15">
+        <v>927369</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="17">
+        <v>8661070</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F24">
-        <v>-77.784972999999994</v>
-      </c>
-      <c r="G24">
-        <v>34.21331</v>
-      </c>
-      <c r="H24">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I24">
-        <v>0.17069999999999999</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="F27" s="17">
+        <v>-78.916383999999994</v>
+      </c>
+      <c r="G27" s="17">
+        <v>33.655000000000001</v>
+      </c>
+      <c r="H27" s="17">
+        <v>0.45</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0.13719999999999999</v>
+      </c>
+      <c r="J27" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="2">
-        <v>-77.784972999999994</v>
-      </c>
-      <c r="L24" s="2">
-        <v>34.21331</v>
-      </c>
-      <c r="M24">
-        <v>2.5758999999999999</v>
-      </c>
-      <c r="N24">
-        <v>1859231</v>
-      </c>
-      <c r="O24">
-        <v>927369</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="K27" s="18">
+        <v>-78.909931</v>
+      </c>
+      <c r="L27" s="18">
+        <v>33.641724000000004</v>
+      </c>
+      <c r="M27" s="17">
+        <v>7.0872999999999999</v>
+      </c>
+      <c r="N27" s="17">
+        <v>1840490</v>
+      </c>
+      <c r="O27" s="17">
+        <v>913115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="15">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="17">
+        <v>8665530</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="17">
+        <v>-79.922178000000002</v>
+      </c>
+      <c r="G28" s="17">
+        <v>32.781700000000001</v>
+      </c>
+      <c r="H28" s="17">
+        <v>0.22</v>
+      </c>
+      <c r="I28" s="17">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="J28" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="4">
-        <v>8661070</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="K28" s="18">
+        <v>-79.861604495927807</v>
+      </c>
+      <c r="L28" s="18">
+        <v>32.7438895845399</v>
+      </c>
+      <c r="M28" s="17">
+        <v>11.473000000000001</v>
+      </c>
+      <c r="N28" s="17">
+        <v>1821427</v>
+      </c>
+      <c r="O28" s="17">
+        <v>908263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="15">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="17">
+        <v>8670870</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="4">
-        <v>-78.916383999999994</v>
-      </c>
-      <c r="G25" s="4">
-        <v>33.655000000000001</v>
-      </c>
-      <c r="H25" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0.13719999999999999</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="F29" s="17">
+        <v>-80.901700000000005</v>
+      </c>
+      <c r="G29" s="17">
+        <v>32.034612000000003</v>
+      </c>
+      <c r="H29" s="17">
+        <v>0.23</v>
+      </c>
+      <c r="I29" s="17">
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="J29" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="5">
-        <v>-78.909931</v>
-      </c>
-      <c r="L25" s="5">
-        <v>33.641724000000004</v>
-      </c>
-      <c r="M25" s="4">
-        <v>7.0872999999999999</v>
-      </c>
-      <c r="N25" s="4">
-        <v>1840490</v>
-      </c>
-      <c r="O25" s="4">
-        <v>913115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>24</v>
-      </c>
-      <c r="B26" s="4">
-        <v>8665530</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="4">
-        <v>-79.922178000000002</v>
-      </c>
-      <c r="G26" s="4">
-        <v>32.781700000000001</v>
-      </c>
-      <c r="H26" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="I26" s="4">
-        <v>6.7100000000000007E-2</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K26" s="5">
-        <v>-79.861604495927807</v>
-      </c>
-      <c r="L26" s="5">
-        <v>32.7438895845399</v>
-      </c>
-      <c r="M26" s="4">
-        <v>11.473000000000001</v>
-      </c>
-      <c r="N26" s="4">
-        <v>1821427</v>
-      </c>
-      <c r="O26" s="4">
-        <v>908263</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4">
-        <v>8670870</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="4">
-        <v>-80.901700000000005</v>
-      </c>
-      <c r="G27" s="4">
-        <v>32.034612000000003</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0.23</v>
-      </c>
-      <c r="I27" s="4">
-        <v>7.0099999999999996E-2</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="5">
+      <c r="K29" s="18">
         <v>-80.892552488084704</v>
       </c>
-      <c r="L27" s="5">
+      <c r="L29" s="18">
         <v>32.048645051476797</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M29" s="17">
         <v>8.3546999999999993</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N29" s="17">
         <v>1982522</v>
       </c>
-      <c r="O27" s="4">
+      <c r="O29" s="17">
         <v>989537</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K30" s="2"/>
+    <row r="30" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K31" s="2"/>
+      <c r="K31" s="16"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K32" s="2"/>
+      <c r="K32" s="16"/>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K33" s="2"/>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K34" s="16"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K35" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6104,32 +6254,32 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
-        <f>Region3_Stations_V1!K18</f>
+        <f>Region3_Stations_V1!K20</f>
         <v>-75.119159999999994</v>
       </c>
       <c r="B17" s="8">
-        <f>Region3_Stations_V1!L18</f>
+        <f>Region3_Stations_V1!L20</f>
         <v>38.785755999999999</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D17" s="6">
-        <f>Region3_Stations_V1!B18</f>
+        <f>Region3_Stations_V1!B20</f>
         <v>8557380</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F17" s="6" t="str">
-        <f>Region3_Stations_V1!C18</f>
+        <f>Region3_Stations_V1!C20</f>
         <v>Lewes</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H17" s="6" t="str">
-        <f>Region3_Stations_V1!D18</f>
+        <f>Region3_Stations_V1!D20</f>
         <v>DE</v>
       </c>
       <c r="I17" s="7" t="s">
@@ -6141,32 +6291,32 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
-        <f>Region3_Stations_V1!K19</f>
+        <f>Region3_Stations_V1!K21</f>
         <v>-75.091669999999993</v>
       </c>
       <c r="B18" s="8">
-        <f>Region3_Stations_V1!L19</f>
+        <f>Region3_Stations_V1!L21</f>
         <v>38.328330000000001</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D18" s="6">
-        <f>Region3_Stations_V1!B19</f>
+        <f>Region3_Stations_V1!B21</f>
         <v>8570283</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F18" s="6" t="str">
-        <f>Region3_Stations_V1!C19</f>
+        <f>Region3_Stations_V1!C21</f>
         <v>Ocean City Inlet</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H18" s="6" t="str">
-        <f>Region3_Stations_V1!D19</f>
+        <f>Region3_Stations_V1!D21</f>
         <v>MD</v>
       </c>
       <c r="I18" s="7" t="s">
@@ -6178,32 +6328,32 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
-        <f>Region3_Stations_V1!K20</f>
+        <f>Region3_Stations_V1!K22</f>
         <v>-76.5</v>
       </c>
       <c r="B19" s="8">
-        <f>Region3_Stations_V1!L20</f>
+        <f>Region3_Stations_V1!L22</f>
         <v>38</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D19" s="6">
-        <f>Region3_Stations_V1!B20</f>
+        <f>Region3_Stations_V1!B22</f>
         <v>8635750</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F19" s="6" t="str">
-        <f>Region3_Stations_V1!C20</f>
+        <f>Region3_Stations_V1!C22</f>
         <v>Lewisetta</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H19" s="6" t="str">
-        <f>Region3_Stations_V1!D20</f>
+        <f>Region3_Stations_V1!D22</f>
         <v>VA</v>
       </c>
       <c r="I19" s="7" t="s">
@@ -6215,32 +6365,32 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
-        <f>Region3_Stations_V1!K21</f>
+        <f>Region3_Stations_V1!K23</f>
         <v>-76.083332999999996</v>
       </c>
       <c r="B20" s="8">
-        <f>Region3_Stations_V1!L21</f>
+        <f>Region3_Stations_V1!L23</f>
         <v>37.033332999999999</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D20" s="6">
-        <f>Region3_Stations_V1!B21</f>
+        <f>Region3_Stations_V1!B23</f>
         <v>8638901</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F20" s="6" t="str">
-        <f>Region3_Stations_V1!C21</f>
+        <f>Region3_Stations_V1!C23</f>
         <v>CBBT Chesapeake Channel</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H20" s="6" t="str">
-        <f>Region3_Stations_V1!D21</f>
+        <f>Region3_Stations_V1!D23</f>
         <v>VA</v>
       </c>
       <c r="I20" s="7" t="s">
@@ -6252,32 +6402,32 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
-        <f>Region3_Stations_V1!K22</f>
+        <f>Region3_Stations_V1!K24</f>
         <v>-75.746669999999995</v>
       </c>
       <c r="B21" s="8">
-        <f>Region3_Stations_V1!L22</f>
+        <f>Region3_Stations_V1!L24</f>
         <v>36.183329999999998</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D21" s="6">
-        <f>Region3_Stations_V1!B22</f>
+        <f>Region3_Stations_V1!B24</f>
         <v>8651370</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F21" s="6" t="str">
-        <f>Region3_Stations_V1!C22</f>
+        <f>Region3_Stations_V1!C24</f>
         <v>Duck Pier</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H21" s="6" t="str">
-        <f>Region3_Stations_V1!D22</f>
+        <f>Region3_Stations_V1!D24</f>
         <v>NC</v>
       </c>
       <c r="I21" s="7" t="s">
@@ -6289,32 +6439,32 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
-        <f>Region3_Stations_V1!K23</f>
+        <f>Region3_Stations_V1!K25</f>
         <v>-76.672932000000003</v>
       </c>
       <c r="B22" s="8">
-        <f>Region3_Stations_V1!L23</f>
+        <f>Region3_Stations_V1!L25</f>
         <v>34.699781000000002</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D22" s="6">
-        <f>Region3_Stations_V1!B23</f>
+        <f>Region3_Stations_V1!B25</f>
         <v>8656483</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F22" s="6" t="str">
-        <f>Region3_Stations_V1!C23</f>
+        <f>Region3_Stations_V1!C25</f>
         <v>Beaufort</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H22" s="6" t="str">
-        <f>Region3_Stations_V1!D23</f>
+        <f>Region3_Stations_V1!D25</f>
         <v>NC</v>
       </c>
       <c r="I22" s="7" t="s">
@@ -6326,32 +6476,32 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
-        <f>Region3_Stations_V1!K24</f>
+        <f>Region3_Stations_V1!K26</f>
         <v>-77.784972999999994</v>
       </c>
       <c r="B23" s="8">
-        <f>Region3_Stations_V1!L24</f>
+        <f>Region3_Stations_V1!L26</f>
         <v>34.21331</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D23" s="6">
-        <f>Region3_Stations_V1!B24</f>
+        <f>Region3_Stations_V1!B26</f>
         <v>8658163</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F23" s="6" t="str">
-        <f>Region3_Stations_V1!C24</f>
+        <f>Region3_Stations_V1!C26</f>
         <v>Wrightsville Beach</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H23" s="6" t="str">
-        <f>Region3_Stations_V1!D24</f>
+        <f>Region3_Stations_V1!D26</f>
         <v>NC</v>
       </c>
       <c r="I23" s="7" t="s">
@@ -6363,32 +6513,32 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
-        <f>Region3_Stations_V1!K25</f>
+        <f>Region3_Stations_V1!K27</f>
         <v>-78.909931</v>
       </c>
       <c r="B24" s="8">
-        <f>Region3_Stations_V1!L25</f>
+        <f>Region3_Stations_V1!L27</f>
         <v>33.641724000000004</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D24" s="6">
-        <f>Region3_Stations_V1!B25</f>
+        <f>Region3_Stations_V1!B27</f>
         <v>8661070</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F24" s="6" t="str">
-        <f>Region3_Stations_V1!C25</f>
+        <f>Region3_Stations_V1!C27</f>
         <v>Springmaid Pier</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H24" s="6" t="str">
-        <f>Region3_Stations_V1!D25</f>
+        <f>Region3_Stations_V1!D27</f>
         <v>SC</v>
       </c>
       <c r="I24" s="7" t="s">
@@ -6400,32 +6550,32 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
-        <f>Region3_Stations_V1!K26</f>
+        <f>Region3_Stations_V1!K28</f>
         <v>-79.861604495927807</v>
       </c>
       <c r="B25" s="8">
-        <f>Region3_Stations_V1!L26</f>
+        <f>Region3_Stations_V1!L28</f>
         <v>32.7438895845399</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D25" s="6">
-        <f>Region3_Stations_V1!B26</f>
+        <f>Region3_Stations_V1!B28</f>
         <v>8665530</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F25" s="6" t="str">
-        <f>Region3_Stations_V1!C26</f>
+        <f>Region3_Stations_V1!C28</f>
         <v>Charleston Harbor</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H25" s="6" t="str">
-        <f>Region3_Stations_V1!D26</f>
+        <f>Region3_Stations_V1!D28</f>
         <v>SC</v>
       </c>
       <c r="I25" s="7" t="s">
@@ -6437,32 +6587,32 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
-        <f>Region3_Stations_V1!K27</f>
+        <f>Region3_Stations_V1!K29</f>
         <v>-80.892552488084704</v>
       </c>
       <c r="B26" s="8">
-        <f>Region3_Stations_V1!L27</f>
+        <f>Region3_Stations_V1!L29</f>
         <v>32.048645051476797</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D26" s="6">
-        <f>Region3_Stations_V1!B27</f>
+        <f>Region3_Stations_V1!B29</f>
         <v>8670870</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F26" s="6" t="str">
-        <f>Region3_Stations_V1!C27</f>
+        <f>Region3_Stations_V1!C29</f>
         <v>Fort Pulaski</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H26" s="6" t="str">
-        <f>Region3_Stations_V1!D27</f>
+        <f>Region3_Stations_V1!D29</f>
         <v>GA</v>
       </c>
       <c r="I26" s="7" t="s">
@@ -6481,7 +6631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A74D0D5-30C6-344F-9A4C-13EAC440B852}">
   <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A89" activeCellId="24" sqref="A3:XFD3 A6:XFD6 A8:XFD8 A10:XFD10 A13:XFD13 A17:XFD17 A19:XFD19 A25:XFD25 A27:XFD27 A29:XFD29 A31:XFD31 A33:XFD33 A38:XFD38 A40:XFD40 A42:XFD42 A52:XFD52 A54:XFD54 A67:XFD67 A72:XFD72 A75:XFD75 A79:XFD79 A82:XFD82 A84:XFD84 A87:XFD87 A89:XFD89"/>
     </sheetView>
   </sheetViews>
@@ -7702,32 +7852,32 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
-        <f>Region3_Stations_V1!K18</f>
+        <f>Region3_Stations_V1!K20</f>
         <v>-75.119159999999994</v>
       </c>
       <c r="B37" s="8">
-        <f>Region3_Stations_V1!L18</f>
+        <f>Region3_Stations_V1!L20</f>
         <v>38.785755999999999</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D37" s="6">
-        <f>Region3_Stations_V1!B18</f>
+        <f>Region3_Stations_V1!B20</f>
         <v>8557380</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F37" s="6" t="str">
-        <f>Region3_Stations_V1!C18</f>
+        <f>Region3_Stations_V1!C20</f>
         <v>Lewes</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H37" s="6" t="str">
-        <f>Region3_Stations_V1!D18</f>
+        <f>Region3_Stations_V1!D20</f>
         <v>DE</v>
       </c>
       <c r="I37" s="7" t="s">
@@ -7739,32 +7889,32 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
-        <f>Region3_Stations_V1!K19</f>
+        <f>Region3_Stations_V1!K21</f>
         <v>-75.091669999999993</v>
       </c>
       <c r="B38" s="8">
-        <f>Region3_Stations_V1!L19</f>
+        <f>Region3_Stations_V1!L21</f>
         <v>38.328330000000001</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D38" s="6">
-        <f>Region3_Stations_V1!B19</f>
+        <f>Region3_Stations_V1!B21</f>
         <v>8570283</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F38" s="6" t="str">
-        <f>Region3_Stations_V1!C19</f>
+        <f>Region3_Stations_V1!C21</f>
         <v>Ocean City Inlet</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H38" s="6" t="str">
-        <f>Region3_Stations_V1!D19</f>
+        <f>Region3_Stations_V1!D21</f>
         <v>MD</v>
       </c>
       <c r="I38" s="7" t="s">
@@ -8128,32 +8278,32 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
-        <f>Region3_Stations_V1!K20</f>
+        <f>Region3_Stations_V1!K22</f>
         <v>-76.5</v>
       </c>
       <c r="B50" s="8">
-        <f>Region3_Stations_V1!L20</f>
+        <f>Region3_Stations_V1!L22</f>
         <v>38</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D50" s="6">
-        <f>Region3_Stations_V1!B20</f>
+        <f>Region3_Stations_V1!B22</f>
         <v>8635750</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F50" s="6" t="str">
-        <f>Region3_Stations_V1!C20</f>
+        <f>Region3_Stations_V1!C22</f>
         <v>Lewisetta</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H50" s="6" t="str">
-        <f>Region3_Stations_V1!D20</f>
+        <f>Region3_Stations_V1!D22</f>
         <v>VA</v>
       </c>
       <c r="I50" s="7" t="s">
@@ -8261,32 +8411,32 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
-        <f>Region3_Stations_V1!K21</f>
+        <f>Region3_Stations_V1!K23</f>
         <v>-76.083332999999996</v>
       </c>
       <c r="B54" s="8">
-        <f>Region3_Stations_V1!L21</f>
+        <f>Region3_Stations_V1!L23</f>
         <v>37.033332999999999</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D54" s="6">
-        <f>Region3_Stations_V1!B21</f>
+        <f>Region3_Stations_V1!B23</f>
         <v>8638901</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F54" s="6" t="str">
-        <f>Region3_Stations_V1!C21</f>
+        <f>Region3_Stations_V1!C23</f>
         <v>CBBT Chesapeake Channel</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H54" s="6" t="str">
-        <f>Region3_Stations_V1!D21</f>
+        <f>Region3_Stations_V1!D23</f>
         <v>VA</v>
       </c>
       <c r="I54" s="7" t="s">
@@ -8330,32 +8480,32 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
-        <f>Region3_Stations_V1!K22</f>
+        <f>Region3_Stations_V1!K24</f>
         <v>-75.746669999999995</v>
       </c>
       <c r="B56" s="8">
-        <f>Region3_Stations_V1!L22</f>
+        <f>Region3_Stations_V1!L24</f>
         <v>36.183329999999998</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D56" s="6">
-        <f>Region3_Stations_V1!B22</f>
+        <f>Region3_Stations_V1!B24</f>
         <v>8651370</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F56" s="6" t="str">
-        <f>Region3_Stations_V1!C22</f>
+        <f>Region3_Stations_V1!C24</f>
         <v>Duck Pier</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H56" s="6" t="str">
-        <f>Region3_Stations_V1!D22</f>
+        <f>Region3_Stations_V1!D24</f>
         <v>NC</v>
       </c>
       <c r="I56" s="7" t="s">
@@ -8431,32 +8581,32 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
-        <f>Region3_Stations_V1!K23</f>
+        <f>Region3_Stations_V1!K25</f>
         <v>-76.672932000000003</v>
       </c>
       <c r="B59" s="8">
-        <f>Region3_Stations_V1!L23</f>
+        <f>Region3_Stations_V1!L25</f>
         <v>34.699781000000002</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D59" s="6">
-        <f>Region3_Stations_V1!B23</f>
+        <f>Region3_Stations_V1!B25</f>
         <v>8656483</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F59" s="6" t="str">
-        <f>Region3_Stations_V1!C23</f>
+        <f>Region3_Stations_V1!C25</f>
         <v>Beaufort</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H59" s="6" t="str">
-        <f>Region3_Stations_V1!D23</f>
+        <f>Region3_Stations_V1!D25</f>
         <v>NC</v>
       </c>
       <c r="I59" s="7" t="s">
@@ -8500,32 +8650,32 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
-        <f>Region3_Stations_V1!K24</f>
+        <f>Region3_Stations_V1!K26</f>
         <v>-77.784972999999994</v>
       </c>
       <c r="B61" s="8">
-        <f>Region3_Stations_V1!L24</f>
+        <f>Region3_Stations_V1!L26</f>
         <v>34.21331</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D61" s="6">
-        <f>Region3_Stations_V1!B24</f>
+        <f>Region3_Stations_V1!B26</f>
         <v>8658163</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F61" s="6" t="str">
-        <f>Region3_Stations_V1!C24</f>
+        <f>Region3_Stations_V1!C26</f>
         <v>Wrightsville Beach</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H61" s="6" t="str">
-        <f>Region3_Stations_V1!D24</f>
+        <f>Region3_Stations_V1!D26</f>
         <v>NC</v>
       </c>
       <c r="I61" s="7" t="s">
@@ -8537,32 +8687,32 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
-        <f>Region3_Stations_V1!K25</f>
+        <f>Region3_Stations_V1!K27</f>
         <v>-78.909931</v>
       </c>
       <c r="B62" s="8">
-        <f>Region3_Stations_V1!L25</f>
+        <f>Region3_Stations_V1!L27</f>
         <v>33.641724000000004</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D62" s="6">
-        <f>Region3_Stations_V1!B25</f>
+        <f>Region3_Stations_V1!B27</f>
         <v>8661070</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F62" s="6" t="str">
-        <f>Region3_Stations_V1!C25</f>
+        <f>Region3_Stations_V1!C27</f>
         <v>Springmaid Pier</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H62" s="6" t="str">
-        <f>Region3_Stations_V1!D25</f>
+        <f>Region3_Stations_V1!D27</f>
         <v>SC</v>
       </c>
       <c r="I62" s="7" t="s">
@@ -8606,32 +8756,32 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
-        <f>Region3_Stations_V1!K26</f>
+        <f>Region3_Stations_V1!K28</f>
         <v>-79.861604495927807</v>
       </c>
       <c r="B64" s="8">
-        <f>Region3_Stations_V1!L26</f>
+        <f>Region3_Stations_V1!L28</f>
         <v>32.7438895845399</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D64" s="6">
-        <f>Region3_Stations_V1!B26</f>
+        <f>Region3_Stations_V1!B28</f>
         <v>8665530</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F64" s="6" t="str">
-        <f>Region3_Stations_V1!C26</f>
+        <f>Region3_Stations_V1!C28</f>
         <v>Charleston Harbor</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H64" s="6" t="str">
-        <f>Region3_Stations_V1!D26</f>
+        <f>Region3_Stations_V1!D28</f>
         <v>SC</v>
       </c>
       <c r="I64" s="7" t="s">
@@ -8643,32 +8793,32 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
-        <f>Region3_Stations_V1!K27</f>
+        <f>Region3_Stations_V1!K29</f>
         <v>-80.892552488084704</v>
       </c>
       <c r="B65" s="8">
-        <f>Region3_Stations_V1!L27</f>
+        <f>Region3_Stations_V1!L29</f>
         <v>32.048645051476797</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D65" s="6">
-        <f>Region3_Stations_V1!B27</f>
+        <f>Region3_Stations_V1!B29</f>
         <v>8670870</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F65" s="6" t="str">
-        <f>Region3_Stations_V1!C27</f>
+        <f>Region3_Stations_V1!C29</f>
         <v>Fort Pulaski</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H65" s="6" t="str">
-        <f>Region3_Stations_V1!D27</f>
+        <f>Region3_Stations_V1!D29</f>
         <v>GA</v>
       </c>
       <c r="I65" s="7" t="s">

</xml_diff>